<commit_message>
TN. 2035. RES updated
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee9/ieee9_2030.xlsx
+++ b/data/IEEE9/ieee9/ieee9_2030.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6D2497-1101-47E6-99FD-07303948ADD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE6DE92-B4EA-4800-964C-4C461D6B949F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26865" yWindow="3390" windowWidth="21600" windowHeight="12660" tabRatio="722" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="3270" windowWidth="28800" windowHeight="15435" tabRatio="722" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>

</xml_diff>